<commit_message>
update Chinese travelers' effects
</commit_message>
<xml_diff>
--- a/result/cn_aireffect.xlsx
+++ b/result/cn_aireffect.xlsx
@@ -519,7 +519,7 @@
         <v>86828.1781021901</v>
       </c>
       <c r="E2">
-        <v>11.37168648048042</v>
+        <v>11.37169799741263</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -610,10 +610,8 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E3">
+        <v>0</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -705,7 +703,7 @@
         <v>178744.7075518089</v>
       </c>
       <c r="E4">
-        <v>12.09371385201616</v>
+        <v>12.09371944657175</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -797,7 +795,7 @@
         <v>3037815.47405249</v>
       </c>
       <c r="E5">
-        <v>14.92664922100826</v>
+        <v>14.92664955019212</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -889,7 +887,7 @@
         <v>370176.6547961765</v>
       </c>
       <c r="E6">
-        <v>12.82173561607469</v>
+        <v>12.82173831748397</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -981,7 +979,7 @@
         <v>8582394.02694848</v>
       </c>
       <c r="E7">
-        <v>15.96522345666402</v>
+        <v>15.96522357318162</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -1073,7 +1071,7 @@
         <v>224715.3847457626</v>
       </c>
       <c r="E8">
-        <v>12.32258992376802</v>
+        <v>12.32259437383171</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1165,7 +1163,7 @@
         <v>23890.7396875</v>
       </c>
       <c r="E9">
-        <v>10.08124620206322</v>
+        <v>10.08128805840945</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -1257,7 +1255,7 @@
         <v>229952.424328023</v>
       </c>
       <c r="E10">
-        <v>12.34562771576104</v>
+        <v>12.34563206447721</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -1349,7 +1347,7 @@
         <v>8410721.792727094</v>
       </c>
       <c r="E11">
-        <v>15.94501785379868</v>
+        <v>15.94501797269454</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -1441,7 +1439,7 @@
         <v>323572.7499999992</v>
       </c>
       <c r="E12">
-        <v>12.68717925172083</v>
+        <v>12.68718234221116</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -1533,7 +1531,7 @@
         <v>3995987.863247867</v>
       </c>
       <c r="E13">
-        <v>15.20080138152071</v>
+        <v>15.20080163177169</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -1625,7 +1623,7 @@
         <v>55759390.28362726</v>
       </c>
       <c r="E14">
-        <v>17.83655638970158</v>
+        <v>17.83655640763578</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -1717,7 +1715,7 @@
         <v>3616672.969040243</v>
       </c>
       <c r="E15">
-        <v>15.10106509187289</v>
+        <v>15.10106536837006</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1809,7 +1807,7 @@
         <v>139837.1020862902</v>
       </c>
       <c r="E16">
-        <v>11.84823346760749</v>
+        <v>11.84824061875986</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1901,7 +1899,7 @@
         <v>5686806.459410318</v>
       </c>
       <c r="E17">
-        <v>15.55365939360333</v>
+        <v>15.55365956944893</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1993,7 +1991,7 @@
         <v>9897151.416182896</v>
       </c>
       <c r="E18">
-        <v>16.10775753796185</v>
+        <v>16.10775763900102</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -2085,7 +2083,7 @@
         <v>27529.81145617667</v>
       </c>
       <c r="E19">
-        <v>10.22302474944544</v>
+        <v>10.22306107304468</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -2177,7 +2175,7 @@
         <v>341294.4156164654</v>
       </c>
       <c r="E20">
-        <v>12.74050077266444</v>
+        <v>12.74050370268172</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2269,7 +2267,7 @@
         <v>16865081.88302302</v>
       </c>
       <c r="E21">
-        <v>16.64075588167055</v>
+        <v>16.64075594096466</v>
       </c>
       <c r="F21">
         <v>0</v>
@@ -2361,7 +2359,7 @@
         <v>104.2199094834678</v>
       </c>
       <c r="E22">
-        <v>4.646503180966661</v>
+        <v>4.656052536042528</v>
       </c>
       <c r="F22">
         <v>0</v>
@@ -2453,7 +2451,7 @@
         <v>52418653.00046701</v>
       </c>
       <c r="E23">
-        <v>17.77477305923917</v>
+        <v>17.77477307831634</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2545,7 +2543,7 @@
         <v>260513.3314671614</v>
       </c>
       <c r="E24">
-        <v>12.47040931532352</v>
+        <v>12.4704131538913</v>
       </c>
       <c r="F24">
         <v>0</v>
@@ -2637,7 +2635,7 @@
         <v>40461.60000000001</v>
       </c>
       <c r="E25">
-        <v>10.6081086551697</v>
+        <v>10.6081333696556</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -2729,7 +2727,7 @@
         <v>1631204.754072924</v>
       </c>
       <c r="E26">
-        <v>14.30482941270167</v>
+        <v>14.30483002574531</v>
       </c>
       <c r="F26">
         <v>0</v>
@@ -2820,10 +2818,8 @@
       <c r="D27">
         <v>0</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E27">
+        <v>0</v>
       </c>
       <c r="F27">
         <v>0</v>
@@ -2915,7 +2911,7 @@
         <v>163985.232308792</v>
       </c>
       <c r="E28">
-        <v>12.00753165585426</v>
+        <v>12.00753775394576</v>
       </c>
       <c r="F28">
         <v>0</v>
@@ -3007,7 +3003,7 @@
         <v>1385089.188777199</v>
       </c>
       <c r="E29">
-        <v>14.14127509175925</v>
+        <v>14.14127581373416</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -3099,7 +3095,7 @@
         <v>489366.4200319352</v>
       </c>
       <c r="E30">
-        <v>13.10086681307172</v>
+        <v>13.10086885652819</v>
       </c>
       <c r="F30">
         <v>0</v>
@@ -3191,7 +3187,7 @@
         <v>18798.49795511221</v>
       </c>
       <c r="E31">
-        <v>9.841532249621515</v>
+        <v>9.84158544394616</v>
       </c>
       <c r="F31">
         <v>0</v>
@@ -3283,7 +3279,7 @@
         <v>11746403.39186692</v>
       </c>
       <c r="E32">
-        <v>16.27905765738882</v>
+        <v>16.27905774252126</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -3375,7 +3371,7 @@
         <v>31417939.2769633</v>
       </c>
       <c r="E33">
-        <v>17.26288960229343</v>
+        <v>17.26288963412237</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -3467,7 +3463,7 @@
         <v>4281414.992668624</v>
       </c>
       <c r="E34">
-        <v>15.26979411868363</v>
+        <v>15.26979435225125</v>
       </c>
       <c r="F34">
         <v>0</v>
@@ -3558,10 +3554,8 @@
       <c r="D35">
         <v>0</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E35">
+        <v>0</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -3652,10 +3646,8 @@
       <c r="D36">
         <v>0</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E36">
+        <v>0</v>
       </c>
       <c r="F36">
         <v>0</v>
@@ -3747,7 +3739,7 @@
         <v>56421.22219600747</v>
       </c>
       <c r="E37">
-        <v>10.94060064678161</v>
+        <v>10.94061837045188</v>
       </c>
       <c r="F37">
         <v>0</v>
@@ -3839,7 +3831,7 @@
         <v>492934.9333333336</v>
       </c>
       <c r="E38">
-        <v>13.10813246324627</v>
+        <v>13.10813449190952</v>
       </c>
       <c r="F38">
         <v>0</v>
@@ -3931,7 +3923,7 @@
         <v>32904.2715342554</v>
       </c>
       <c r="E39">
-        <v>10.40135776219372</v>
+        <v>10.40138815292289</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -4023,7 +4015,7 @@
         <v>1370285.880376428</v>
       </c>
       <c r="E40">
-        <v>14.13052994784299</v>
+        <v>14.13053067761744</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -4114,10 +4106,8 @@
       <c r="D41">
         <v>0</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E41">
+        <v>0</v>
       </c>
       <c r="F41">
         <v>0</v>
@@ -4209,7 +4199,7 @@
         <v>53113.51551886321</v>
       </c>
       <c r="E42">
-        <v>10.88018670438833</v>
+        <v>10.88020553181062</v>
       </c>
       <c r="F42">
         <v>0</v>
@@ -4301,7 +4291,7 @@
         <v>76479.7425852498</v>
       </c>
       <c r="E43">
-        <v>11.24478118194098</v>
+        <v>11.24479425721332</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -4393,7 +4383,7 @@
         <v>2225749.03125</v>
       </c>
       <c r="E44">
-        <v>14.61560406018928</v>
+        <v>14.61560450947613</v>
       </c>
       <c r="F44">
         <v>0</v>
@@ -4485,7 +4475,7 @@
         <v>35860.02788104088</v>
       </c>
       <c r="E45">
-        <v>10.48737852465578</v>
+        <v>10.48740641046949</v>
       </c>
       <c r="F45">
         <v>0</v>
@@ -4577,7 +4567,7 @@
         <v>22944513.31662214</v>
       </c>
       <c r="E46">
-        <v>16.94858939471761</v>
+        <v>16.94858943830101</v>
       </c>
       <c r="F46">
         <v>0</v>
@@ -4669,7 +4659,7 @@
         <v>108725.2489451063</v>
       </c>
       <c r="E47">
-        <v>11.59657932713998</v>
+        <v>11.5965885245933</v>
       </c>
       <c r="F47">
         <v>0</v>
@@ -4761,7 +4751,7 @@
         <v>2129820.202188184</v>
       </c>
       <c r="E48">
-        <v>14.57154812200448</v>
+        <v>14.57154859152757</v>
       </c>
       <c r="F48">
         <v>0</v>
@@ -4853,7 +4843,7 @@
         <v>2099214.498961433</v>
       </c>
       <c r="E49">
-        <v>14.5570737846066</v>
+        <v>14.55707426097515</v>
       </c>
       <c r="F49">
         <v>0</v>
@@ -4944,10 +4934,8 @@
       <c r="D50">
         <v>0</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E50">
+        <v>0</v>
       </c>
       <c r="F50">
         <v>0</v>
@@ -5039,7 +5027,7 @@
         <v>469835.7907510429</v>
       </c>
       <c r="E51">
-        <v>13.06013853125759</v>
+        <v>13.06014065965852</v>
       </c>
       <c r="F51">
         <v>0</v>
@@ -5131,7 +5119,7 @@
         <v>1334542.440506031</v>
       </c>
       <c r="E52">
-        <v>14.10409904987332</v>
+        <v>14.10409979919353</v>
       </c>
       <c r="F52">
         <v>0</v>
@@ -5222,10 +5210,8 @@
       <c r="D53">
         <v>0</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E53">
+        <v>0</v>
       </c>
       <c r="F53">
         <v>0</v>
@@ -5317,7 +5303,7 @@
         <v>810212.3315344153</v>
       </c>
       <c r="E54">
-        <v>13.60505162999335</v>
+        <v>13.60505286423695</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -5409,7 +5395,7 @@
         <v>13141.70707154742</v>
       </c>
       <c r="E55">
-        <v>9.483546197721301</v>
+        <v>9.483622288441454</v>
       </c>
       <c r="F55">
         <v>0</v>
@@ -5501,7 +5487,7 @@
         <v>103460.9783794091</v>
       </c>
       <c r="E56">
-        <v>11.54694980010867</v>
+        <v>11.54695946554179</v>
       </c>
       <c r="F56">
         <v>0</v>
@@ -5593,7 +5579,7 @@
         <v>502870.9875770294</v>
       </c>
       <c r="E57">
-        <v>13.12808893025337</v>
+        <v>13.12809091883301</v>
       </c>
       <c r="F57">
         <v>0</v>
@@ -5685,7 +5671,7 @@
         <v>1473.073724336982</v>
       </c>
       <c r="E58">
-        <v>7.295106465676531</v>
+        <v>7.295785088009341</v>
       </c>
       <c r="F58">
         <v>0</v>
@@ -5777,7 +5763,7 @@
         <v>216773.1336766222</v>
       </c>
       <c r="E59">
-        <v>12.28660661871284</v>
+        <v>12.28661123181999</v>
       </c>
       <c r="F59">
         <v>0</v>
@@ -5869,7 +5855,7 @@
         <v>7111778.970102485</v>
       </c>
       <c r="E60">
-        <v>15.7772629772484</v>
+        <v>15.77726311786019</v>
       </c>
       <c r="F60">
         <v>0</v>
@@ -5961,7 +5947,7 @@
         <v>1330687.503495658</v>
       </c>
       <c r="E61">
-        <v>14.10120628656241</v>
+        <v>14.10120703805336</v>
       </c>
       <c r="F61">
         <v>0</v>
@@ -6052,10 +6038,8 @@
       <c r="D62">
         <v>0</v>
       </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>-Inf</t>
-        </is>
+      <c r="E62">
+        <v>0</v>
       </c>
       <c r="F62">
         <v>0</v>

</xml_diff>

<commit_message>
update data and plots to March 31th.
</commit_message>
<xml_diff>
--- a/result/cn_aireffect.xlsx
+++ b/result/cn_aireffect.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB65"/>
+  <dimension ref="A1:AH66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,67 +435,97 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
+          <t>ln_confirmed_20200211</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
           <t>ln_confirmed_20200217</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200219</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200221</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>ln_confirmed_20200223</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>ln_confirmed_20200225</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>ln_confirmed_20200227</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200304</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200307</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200310</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200311</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200312</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200314</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>ln_confirmed_20200316</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200318</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200320</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200324</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>ln_confirmed_20200325</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>ln_confirmed_20200331</t>
         </is>
       </c>
     </row>
@@ -570,25 +600,43 @@
         <v>0</v>
       </c>
       <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
         <v>2.564949357461537</v>
       </c>
-      <c r="W2">
+      <c r="AA2">
         <v>2.772588722239781</v>
       </c>
-      <c r="X2">
+      <c r="AB2">
         <v>3.526360524616162</v>
       </c>
-      <c r="Y2">
+      <c r="AC2">
+        <v>3.761200115693562</v>
+      </c>
+      <c r="AD2">
         <v>4.0943445622221</v>
       </c>
-      <c r="Z2">
+      <c r="AE2">
         <v>4.174387269895637</v>
       </c>
-      <c r="AA2">
+      <c r="AF2">
         <v>4.820281565605037</v>
       </c>
-      <c r="AB2">
+      <c r="AG2">
         <v>4.990432586778736</v>
+      </c>
+      <c r="AH2">
+        <v>5.497168225293202</v>
       </c>
     </row>
     <row r="3">
@@ -607,12 +655,6 @@
           <t>Andorra</t>
         </is>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
       <c r="F3">
         <v>0</v>
       </c>
@@ -653,34 +695,52 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T3">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U3">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V3">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W3">
         <v>0.6931471805599453</v>
       </c>
       <c r="X3">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y3">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z3">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA3">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB3">
         <v>1.09861228866811</v>
       </c>
-      <c r="Y3">
+      <c r="AC3">
+        <v>1.791759469228055</v>
+      </c>
+      <c r="AD3">
         <v>3.688879454113936</v>
       </c>
-      <c r="Z3">
+      <c r="AE3">
         <v>4.31748811353631</v>
       </c>
-      <c r="AA3">
+      <c r="AF3">
         <v>5.10594547390058</v>
       </c>
-      <c r="AB3">
+      <c r="AG3">
         <v>5.241747015059643</v>
+      </c>
+      <c r="AH3">
+        <v>5.916202062607435</v>
       </c>
     </row>
     <row r="4">
@@ -745,34 +805,52 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T4">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V4">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W4">
         <v>0.6931471805599453</v>
       </c>
       <c r="X4">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y4">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z4">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA4">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB4">
         <v>2.19722457733622</v>
       </c>
-      <c r="Y4">
+      <c r="AC4">
+        <v>3.433987204485146</v>
+      </c>
+      <c r="AD4">
         <v>4.442651256490317</v>
       </c>
-      <c r="Z4">
+      <c r="AE4">
         <v>4.919980925828125</v>
       </c>
-      <c r="AA4">
+      <c r="AF4">
         <v>5.46383180502561</v>
       </c>
-      <c r="AB4">
+      <c r="AG4">
         <v>5.583496308781699</v>
+      </c>
+      <c r="AH4">
+        <v>6.278521424165844</v>
       </c>
     </row>
     <row r="5">
@@ -837,34 +915,52 @@
         <v>0</v>
       </c>
       <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="W5">
         <v>3.332204510175204</v>
       </c>
-      <c r="T5">
+      <c r="X5">
         <v>4.204692619390966</v>
       </c>
-      <c r="U5">
+      <c r="Y5">
         <v>4.882801922586371</v>
       </c>
-      <c r="V5">
+      <c r="Z5">
         <v>5.332718793265369</v>
       </c>
-      <c r="W5">
+      <c r="AA5">
         <v>5.713732805509369</v>
       </c>
-      <c r="X5">
+      <c r="AB5">
         <v>6.22455842927536</v>
       </c>
-      <c r="Y5">
+      <c r="AC5">
+        <v>6.866933284461882</v>
+      </c>
+      <c r="AD5">
         <v>7.294377299288821</v>
       </c>
-      <c r="Z5">
+      <c r="AE5">
         <v>7.698029170272805</v>
       </c>
-      <c r="AA5">
+      <c r="AF5">
         <v>8.482601746646619</v>
       </c>
-      <c r="AB5">
+      <c r="AG5">
         <v>8.615589513272431</v>
+      </c>
+      <c r="AH5">
+        <v>9.207837241758064</v>
       </c>
     </row>
     <row r="6">
@@ -929,34 +1025,52 @@
         <v>0</v>
       </c>
       <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
         <v>1.386294361119891</v>
       </c>
-      <c r="T6">
+      <c r="X6">
         <v>2.302585092994046</v>
       </c>
-      <c r="U6">
+      <c r="Y6">
         <v>2.484906649788</v>
       </c>
-      <c r="V6">
+      <c r="Z6">
         <v>2.484906649788</v>
       </c>
-      <c r="W6">
+      <c r="AA6">
         <v>2.484906649788</v>
       </c>
-      <c r="X6">
+      <c r="AB6">
         <v>2.995732273553991</v>
       </c>
-      <c r="Y6">
+      <c r="AC6">
+        <v>3.258096538021482</v>
+      </c>
+      <c r="AD6">
         <v>3.367295829986474</v>
       </c>
-      <c r="Z6">
+      <c r="AE6">
         <v>3.80666248977032</v>
       </c>
-      <c r="AA6">
+      <c r="AF6">
         <v>4.290459441148391</v>
       </c>
-      <c r="AB6">
+      <c r="AG6">
         <v>4.477336814478207</v>
+      </c>
+      <c r="AH6">
+        <v>5.700443573390687</v>
       </c>
     </row>
     <row r="7">
@@ -1021,34 +1135,52 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="S7">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="T7">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="U7">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="V7">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W7">
         <v>3.178053830347946</v>
       </c>
-      <c r="T7">
+      <c r="X7">
         <v>4.700480365792417</v>
       </c>
-      <c r="U7">
+      <c r="Y7">
         <v>5.480638923341991</v>
       </c>
-      <c r="V7">
+      <c r="Z7">
         <v>5.752572638825633</v>
       </c>
-      <c r="W7">
+      <c r="AA7">
         <v>5.752572638825633</v>
       </c>
-      <c r="X7">
+      <c r="AB7">
         <v>6.327936783729195</v>
       </c>
-      <c r="Y7">
+      <c r="AC7">
+        <v>6.787844982309579</v>
+      </c>
+      <c r="AD7">
         <v>7.304515946460155</v>
       </c>
-      <c r="Z7">
+      <c r="AE7">
         <v>7.493317248862145</v>
       </c>
-      <c r="AA7">
+      <c r="AF7">
         <v>8.440312147080279</v>
       </c>
-      <c r="AB7">
+      <c r="AG7">
         <v>8.504715669905124</v>
+      </c>
+      <c r="AH7">
+        <v>9.455323689894849</v>
       </c>
     </row>
     <row r="8">
@@ -1119,28 +1251,46 @@
         <v>0</v>
       </c>
       <c r="U8">
+        <v>0</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
         <v>1.6094379124341</v>
       </c>
-      <c r="V8">
+      <c r="Z8">
         <v>1.945910149055313</v>
       </c>
-      <c r="W8">
+      <c r="AA8">
         <v>2.079441541679836</v>
       </c>
-      <c r="X8">
+      <c r="AB8">
         <v>3.433987204485146</v>
       </c>
-      <c r="Y8">
+      <c r="AC8">
+        <v>3.970291913552122</v>
+      </c>
+      <c r="AD8">
         <v>4.406719247264253</v>
       </c>
-      <c r="Z8">
+      <c r="AE8">
         <v>4.727387818712341</v>
       </c>
-      <c r="AA8">
+      <c r="AF8">
         <v>5.313205979041787</v>
       </c>
-      <c r="AB8">
+      <c r="AG8">
         <v>5.398162701517752</v>
+      </c>
+      <c r="AH8">
+        <v>5.940171252720432</v>
       </c>
     </row>
     <row r="9">
@@ -1208,31 +1358,49 @@
         <v>0</v>
       </c>
       <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
         <v>1.386294361119891</v>
       </c>
-      <c r="U9">
-        <v>0</v>
-      </c>
-      <c r="V9">
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
         <v>1.791759469228055</v>
       </c>
-      <c r="W9">
+      <c r="AA9">
         <v>2.484906649788</v>
       </c>
-      <c r="X9">
+      <c r="AB9">
         <v>2.639057329615258</v>
       </c>
-      <c r="Y9">
+      <c r="AC9">
+        <v>3.218875824868201</v>
+      </c>
+      <c r="AD9">
         <v>3.663561646129646</v>
       </c>
-      <c r="Z9">
+      <c r="AE9">
         <v>4.174387269895637</v>
       </c>
-      <c r="AA9">
+      <c r="AF9">
         <v>5.017279836814924</v>
       </c>
-      <c r="AB9">
+      <c r="AG9">
         <v>5.129898714923073</v>
+      </c>
+      <c r="AH9">
+        <v>6.021023349349527</v>
       </c>
     </row>
     <row r="10">
@@ -1297,34 +1465,52 @@
         <v>0</v>
       </c>
       <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>0</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
         <v>1.945910149055313</v>
       </c>
-      <c r="T10">
+      <c r="X10">
         <v>1.945910149055313</v>
       </c>
-      <c r="U10">
+      <c r="Y10">
         <v>2.302585092994046</v>
       </c>
-      <c r="V10">
+      <c r="Z10">
         <v>2.302585092994046</v>
       </c>
-      <c r="W10">
+      <c r="AA10">
         <v>2.564949357461537</v>
       </c>
-      <c r="X10">
+      <c r="AB10">
         <v>3.332204510175204</v>
       </c>
-      <c r="Y10">
+      <c r="AC10">
+        <v>3.332204510175204</v>
+      </c>
+      <c r="AD10">
         <v>3.951243718581428</v>
       </c>
-      <c r="Z10">
+      <c r="AE10">
         <v>4.248495242049359</v>
       </c>
-      <c r="AA10">
+      <c r="AF10">
         <v>4.406719247264253</v>
       </c>
-      <c r="AB10">
+      <c r="AG10">
         <v>4.465908118654584</v>
+      </c>
+      <c r="AH10">
+        <v>5.030437921392435</v>
       </c>
     </row>
     <row r="11">
@@ -1389,34 +1575,52 @@
         <v>0</v>
       </c>
       <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>1.6094379124341</v>
+      </c>
+      <c r="W11">
         <v>4.23410650459726</v>
       </c>
-      <c r="T11">
+      <c r="X11">
         <v>5.370638028127662</v>
       </c>
-      <c r="U11">
+      <c r="Y11">
         <v>5.926926025970411</v>
       </c>
-      <c r="V11">
+      <c r="Z11">
         <v>6.419994928147142</v>
       </c>
-      <c r="W11">
+      <c r="AA11">
         <v>6.481577129276431</v>
       </c>
-      <c r="X11">
+      <c r="AB11">
         <v>7.038783541388542</v>
       </c>
-      <c r="Y11">
+      <c r="AC11">
+        <v>7.704361167910313</v>
+      </c>
+      <c r="AD11">
         <v>7.901377353792616</v>
       </c>
-      <c r="Z11">
+      <c r="AE11">
         <v>8.348301054933943</v>
       </c>
-      <c r="AA11">
+      <c r="AF11">
         <v>9.118005760773388</v>
       </c>
-      <c r="AB11">
+      <c r="AG11">
         <v>9.255026889598589</v>
+      </c>
+      <c r="AH11">
+        <v>9.691345759329694</v>
       </c>
     </row>
     <row r="12">
@@ -1487,28 +1691,46 @@
         <v>0</v>
       </c>
       <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
         <v>1.09861228866811</v>
       </c>
-      <c r="V12">
+      <c r="Z12">
         <v>1.386294361119891</v>
       </c>
-      <c r="W12">
+      <c r="AA12">
         <v>1.945910149055313</v>
       </c>
-      <c r="X12">
+      <c r="AB12">
         <v>2.70805020110221</v>
       </c>
-      <c r="Y12">
+      <c r="AC12">
+        <v>3.526360524616162</v>
+      </c>
+      <c r="AD12">
         <v>3.912023005428146</v>
       </c>
-      <c r="Z12">
+      <c r="AE12">
         <v>4.219507705176107</v>
       </c>
-      <c r="AA12">
+      <c r="AF12">
         <v>4.762173934797756</v>
       </c>
-      <c r="AB12">
+      <c r="AG12">
         <v>4.828313737302302</v>
+      </c>
+      <c r="AH12">
+        <v>5.442417710521793</v>
       </c>
     </row>
     <row r="13">
@@ -1573,34 +1795,52 @@
         <v>0</v>
       </c>
       <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <v>1.791759469228055</v>
       </c>
-      <c r="T13">
+      <c r="X13">
         <v>2.995732273553991</v>
       </c>
-      <c r="U13">
+      <c r="Y13">
         <v>3.663561646129646</v>
       </c>
-      <c r="V13">
+      <c r="Z13">
         <v>4.174387269895637</v>
       </c>
-      <c r="W13">
+      <c r="AA13">
         <v>4.553876891600541</v>
       </c>
-      <c r="X13">
+      <c r="AB13">
         <v>4.955827057601261</v>
       </c>
-      <c r="Y13">
+      <c r="AC13">
+        <v>5.700443573390687</v>
+      </c>
+      <c r="AD13">
         <v>6.142037405587356</v>
       </c>
-      <c r="Z13">
+      <c r="AE13">
         <v>6.652863029353347</v>
       </c>
-      <c r="AA13">
+      <c r="AF13">
         <v>7.162397497355718</v>
       </c>
-      <c r="AB13">
+      <c r="AG13">
         <v>7.311886164077165</v>
+      </c>
+      <c r="AH13">
+        <v>8.00736706798333</v>
       </c>
     </row>
     <row r="14">
@@ -1656,7 +1896,7 @@
         <v>2.70805020110221</v>
       </c>
       <c r="P14">
-        <v>2.833213344056216</v>
+        <v>2.70805020110221</v>
       </c>
       <c r="Q14">
         <v>2.833213344056216</v>
@@ -1665,34 +1905,52 @@
         <v>2.833213344056216</v>
       </c>
       <c r="S14">
+        <v>2.833213344056216</v>
+      </c>
+      <c r="T14">
+        <v>2.833213344056216</v>
+      </c>
+      <c r="U14">
+        <v>2.833213344056216</v>
+      </c>
+      <c r="V14">
+        <v>3.332204510175204</v>
+      </c>
+      <c r="W14">
         <v>5.501258210544727</v>
       </c>
-      <c r="T14">
+      <c r="X14">
         <v>6.508769136971682</v>
       </c>
-      <c r="U14">
+      <c r="Y14">
         <v>7.110696122978827</v>
       </c>
-      <c r="V14">
+      <c r="Z14">
         <v>7.392031567514591</v>
       </c>
-      <c r="W14">
+      <c r="AA14">
         <v>7.639642287858013</v>
       </c>
-      <c r="X14">
+      <c r="AB14">
         <v>8.209580483475577</v>
       </c>
-      <c r="Y14">
+      <c r="AC14">
+        <v>8.668024081118821</v>
+      </c>
+      <c r="AD14">
         <v>9.218606116393214</v>
       </c>
-      <c r="Z14">
+      <c r="AE14">
         <v>9.644716823578767</v>
       </c>
-      <c r="AA14">
+      <c r="AF14">
         <v>10.31397336910116</v>
       </c>
-      <c r="AB14">
+      <c r="AG14">
         <v>10.43576150750799</v>
+      </c>
+      <c r="AH14">
+        <v>11.11322371675117</v>
       </c>
     </row>
     <row r="15">
@@ -1757,34 +2015,52 @@
         <v>0</v>
       </c>
       <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W15">
         <v>2.397895272798371</v>
       </c>
-      <c r="T15">
+      <c r="X15">
         <v>3.178053830347946</v>
       </c>
-      <c r="U15">
+      <c r="Y15">
         <v>4.736198448394496</v>
       </c>
-      <c r="V15">
+      <c r="Z15">
         <v>5.831882477283517</v>
       </c>
-      <c r="W15">
+      <c r="AA15">
         <v>6.423246963533519</v>
       </c>
-      <c r="X15">
+      <c r="AB15">
         <v>6.687108607866515</v>
       </c>
-      <c r="Y15">
+      <c r="AC15">
+        <v>6.80128303447162</v>
+      </c>
+      <c r="AD15">
         <v>6.941190055068374</v>
       </c>
-      <c r="Z15">
+      <c r="AE15">
         <v>7.112327444710911</v>
       </c>
-      <c r="AA15">
+      <c r="AF15">
         <v>7.363913501405819</v>
       </c>
-      <c r="AB15">
+      <c r="AG15">
         <v>7.447751280047908</v>
+      </c>
+      <c r="AH15">
+        <v>7.943072717277933</v>
       </c>
     </row>
     <row r="16">
@@ -1849,34 +2125,52 @@
         <v>0</v>
       </c>
       <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W16">
         <v>1.791759469228055</v>
       </c>
-      <c r="T16">
+      <c r="X16">
         <v>2.890371757896165</v>
       </c>
-      <c r="U16">
+      <c r="Y16">
         <v>3.044522437723423</v>
       </c>
-      <c r="V16">
+      <c r="Z16">
         <v>3.044522437723423</v>
       </c>
-      <c r="W16">
+      <c r="AA16">
         <v>3.218875824868201</v>
       </c>
-      <c r="X16">
+      <c r="AB16">
         <v>3.332204510175204</v>
       </c>
-      <c r="Y16">
+      <c r="AC16">
+        <v>4.007333185232471</v>
+      </c>
+      <c r="AD16">
         <v>4.290459441148391</v>
       </c>
-      <c r="Z16">
+      <c r="AE16">
         <v>4.51085950651685</v>
       </c>
-      <c r="AA16">
+      <c r="AF16">
         <v>5.442417710521793</v>
       </c>
-      <c r="AB16">
+      <c r="AG16">
         <v>5.579729825986222</v>
+      </c>
+      <c r="AH16">
+        <v>6.371611847231857</v>
       </c>
     </row>
     <row r="17">
@@ -1931,9 +2225,6 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17">
-        <v>0.6931471805599453</v>
-      </c>
       <c r="Q17">
         <v>0.6931471805599453</v>
       </c>
@@ -1941,34 +2232,52 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="S17">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="T17">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="U17">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="V17">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W17">
         <v>1.09861228866811</v>
       </c>
-      <c r="T17">
+      <c r="X17">
         <v>2.772588722239781</v>
       </c>
-      <c r="U17">
+      <c r="Y17">
         <v>4.0943445622221</v>
       </c>
-      <c r="V17">
+      <c r="Z17">
         <v>4.0943445622221</v>
       </c>
-      <c r="W17">
+      <c r="AA17">
         <v>4.219507705176107</v>
       </c>
-      <c r="X17">
+      <c r="AB17">
         <v>4.543294782270004</v>
       </c>
-      <c r="Y17">
+      <c r="AC17">
+        <v>4.844187086458591</v>
+      </c>
+      <c r="AD17">
         <v>5.283203728737988</v>
       </c>
-      <c r="Z17">
+      <c r="AE17">
         <v>5.54907608489522</v>
       </c>
-      <c r="AA17">
+      <c r="AF17">
         <v>5.905361848054571</v>
       </c>
-      <c r="AB17">
+      <c r="AG17">
         <v>5.998936561946683</v>
+      </c>
+      <c r="AH17">
+        <v>6.48768401848461</v>
       </c>
     </row>
     <row r="18">
@@ -2033,34 +2342,52 @@
         <v>1.09861228866811</v>
       </c>
       <c r="S18">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="T18">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="U18">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="V18">
+        <v>2.772588722239781</v>
+      </c>
+      <c r="W18">
         <v>5.267858159063328</v>
       </c>
-      <c r="T18">
+      <c r="X18">
         <v>5.996452088619021</v>
       </c>
-      <c r="U18">
+      <c r="Y18">
         <v>7.116394144093465</v>
       </c>
-      <c r="V18">
+      <c r="Z18">
         <v>7.614312146452</v>
       </c>
-      <c r="W18">
+      <c r="AA18">
         <v>7.731053144007127</v>
       </c>
-      <c r="X18">
+      <c r="AB18">
         <v>8.562740006372207</v>
       </c>
-      <c r="Y18">
+      <c r="AC18">
+        <v>8.985820874482043</v>
+      </c>
+      <c r="AD18">
         <v>9.531336323457896</v>
       </c>
-      <c r="Z18">
+      <c r="AE18">
         <v>9.802451008358355</v>
       </c>
-      <c r="AA18">
+      <c r="AF18">
         <v>10.58845134028805</v>
       </c>
-      <c r="AB18">
+      <c r="AG18">
         <v>10.77081910595874</v>
+      </c>
+      <c r="AH18">
+        <v>11.45548701192296</v>
       </c>
     </row>
     <row r="19">
@@ -2125,34 +2452,52 @@
         <v>0</v>
       </c>
       <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W19">
         <v>1.09861228866811</v>
       </c>
-      <c r="T19">
+      <c r="X19">
         <v>2.397895272798371</v>
       </c>
-      <c r="U19">
+      <c r="Y19">
         <v>2.397895272798371</v>
       </c>
-      <c r="V19">
+      <c r="Z19">
         <v>2.639057329615258</v>
       </c>
-      <c r="W19">
+      <c r="AA19">
         <v>2.833213344056216</v>
       </c>
-      <c r="X19">
+      <c r="AB19">
         <v>4.382026634673881</v>
       </c>
-      <c r="Y19">
+      <c r="AC19">
+        <v>5.147494476813453</v>
+      </c>
+      <c r="AD19">
         <v>5.556828061699537</v>
       </c>
-      <c r="Z19">
+      <c r="AE19">
         <v>5.590986980510857</v>
       </c>
-      <c r="AA19">
+      <c r="AF19">
         <v>5.91350300563827</v>
       </c>
-      <c r="AB19">
+      <c r="AG19">
         <v>6.003887067106539</v>
+      </c>
+      <c r="AH19">
+        <v>6.61472560020376</v>
       </c>
     </row>
     <row r="20">
@@ -2217,34 +2562,52 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="S20">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="T20">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="U20">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="V20">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="W20">
         <v>2.079441541679836</v>
       </c>
-      <c r="T20">
+      <c r="X20">
         <v>2.772588722239781</v>
       </c>
-      <c r="U20">
+      <c r="Y20">
         <v>3.526360524616162</v>
       </c>
-      <c r="V20">
+      <c r="Z20">
         <v>4.07753744390572</v>
       </c>
-      <c r="W20">
+      <c r="AA20">
         <v>1.386294361119891</v>
       </c>
-      <c r="X20">
+      <c r="AB20">
         <v>1.791759469228055</v>
       </c>
-      <c r="Y20">
+      <c r="AC20">
+        <v>2.564949357461537</v>
+      </c>
+      <c r="AD20">
         <v>3.58351893845611</v>
       </c>
-      <c r="Z20">
+      <c r="AE20">
         <v>3.871201010907891</v>
       </c>
-      <c r="AA20">
+      <c r="AF20">
         <v>4.477336814478207</v>
       </c>
-      <c r="AB20">
+      <c r="AG20">
         <v>4.543294782270004</v>
+      </c>
+      <c r="AH20">
+        <v>4.700480365792417</v>
       </c>
     </row>
     <row r="21">
@@ -2300,43 +2663,61 @@
         <v>2.484906649788</v>
       </c>
       <c r="P21">
-        <v>0</v>
+        <v>2.484906649788</v>
       </c>
       <c r="Q21">
-        <v>2.564949357461537</v>
+        <v>0</v>
       </c>
       <c r="R21">
         <v>2.564949357461537</v>
       </c>
       <c r="S21">
+        <v>2.564949357461537</v>
+      </c>
+      <c r="T21">
+        <v>2.564949357461537</v>
+      </c>
+      <c r="U21">
+        <v>2.564949357461537</v>
+      </c>
+      <c r="V21">
+        <v>2.94443897916644</v>
+      </c>
+      <c r="W21">
         <v>5.361292165709425</v>
       </c>
-      <c r="T21">
+      <c r="X21">
         <v>6.493753839851686</v>
       </c>
-      <c r="U21">
+      <c r="Y21">
         <v>7.26403014289953</v>
       </c>
-      <c r="V21">
+      <c r="Z21">
         <v>7.491645473605133</v>
       </c>
-      <c r="W21">
+      <c r="AA21">
         <v>7.736743682453495</v>
       </c>
-      <c r="X21">
+      <c r="AB21">
         <v>8.210668031162976</v>
       </c>
-      <c r="Y21">
+      <c r="AC21">
+        <v>8.605936401250625</v>
+      </c>
+      <c r="AD21">
         <v>8.957510510291613</v>
       </c>
-      <c r="Z21">
+      <c r="AE21">
         <v>9.31542084842669</v>
       </c>
-      <c r="AA21">
+      <c r="AF21">
         <v>9.934259211202882</v>
       </c>
-      <c r="AB21">
+      <c r="AG21">
         <v>10.02517407079273</v>
+      </c>
+      <c r="AH21">
+        <v>10.71745758826044</v>
       </c>
     </row>
     <row r="22">
@@ -2401,34 +2782,52 @@
         <v>0</v>
       </c>
       <c r="S22">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T22">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U22">
         <v>0</v>
       </c>
       <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X22">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
         <v>1.09861228866811</v>
       </c>
-      <c r="W22">
+      <c r="AA22">
         <v>1.09861228866811</v>
       </c>
-      <c r="X22">
+      <c r="AB22">
         <v>1.386294361119891</v>
       </c>
-      <c r="Y22">
+      <c r="AC22">
+        <v>2.484906649788</v>
+      </c>
+      <c r="AD22">
         <v>4.07753744390572</v>
       </c>
-      <c r="Z22">
+      <c r="AE22">
         <v>4.394449154672439</v>
       </c>
-      <c r="AA22">
+      <c r="AF22">
         <v>4.812184355372417</v>
       </c>
-      <c r="AB22">
+      <c r="AG22">
         <v>4.890349128221754</v>
+      </c>
+      <c r="AH22">
+        <v>5.135798437050262</v>
       </c>
     </row>
     <row r="23">
@@ -2484,7 +2883,7 @@
         <v>2.19722457733622</v>
       </c>
       <c r="P23">
-        <v>2.302585092994046</v>
+        <v>2.19722457733622</v>
       </c>
       <c r="Q23">
         <v>2.302585092994046</v>
@@ -2493,34 +2892,52 @@
         <v>2.302585092994046</v>
       </c>
       <c r="S23">
+        <v>2.302585092994046</v>
+      </c>
+      <c r="T23">
+        <v>2.302585092994046</v>
+      </c>
+      <c r="U23">
+        <v>2.639057329615258</v>
+      </c>
+      <c r="V23">
+        <v>2.772588722239781</v>
+      </c>
+      <c r="W23">
         <v>3.988984046564275</v>
       </c>
-      <c r="T23">
+      <c r="X23">
         <v>5.10594547390058</v>
       </c>
-      <c r="U23">
+      <c r="Y23">
         <v>5.774551545544409</v>
       </c>
-      <c r="V23">
+      <c r="Z23">
         <v>5.948034989180646</v>
       </c>
-      <c r="W23">
+      <c r="AA23">
         <v>6.124683390894205</v>
       </c>
-      <c r="X23">
+      <c r="AB23">
         <v>6.683360945766275</v>
       </c>
-      <c r="Y23">
+      <c r="AC23">
+        <v>7.241366283322318</v>
+      </c>
+      <c r="AD23">
         <v>7.577121930876679</v>
       </c>
-      <c r="Z23">
+      <c r="AE23">
         <v>8.092545263891299</v>
       </c>
-      <c r="AA23">
+      <c r="AF23">
         <v>8.802522498284421</v>
       </c>
-      <c r="AB23">
+      <c r="AG23">
         <v>9.015298250772847</v>
+      </c>
+      <c r="AH23">
+        <v>10.01036691416322</v>
       </c>
     </row>
     <row r="24">
@@ -2585,34 +3002,52 @@
         <v>0</v>
       </c>
       <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W24">
         <v>1.386294361119891</v>
       </c>
-      <c r="T24">
+      <c r="X24">
         <v>1.6094379124341</v>
       </c>
-      <c r="U24">
+      <c r="Y24">
         <v>2.772588722239781</v>
       </c>
-      <c r="V24">
+      <c r="Z24">
         <v>3.178053830347946</v>
       </c>
-      <c r="W24">
+      <c r="AA24">
         <v>3.218875824868201</v>
       </c>
-      <c r="X24">
+      <c r="AB24">
         <v>3.258096538021482</v>
       </c>
-      <c r="Y24">
+      <c r="AC24">
+        <v>3.526360524616162</v>
+      </c>
+      <c r="AD24">
         <v>3.663561646129646</v>
       </c>
-      <c r="Z24">
+      <c r="AE24">
         <v>3.784189633918261</v>
       </c>
-      <c r="AA24">
+      <c r="AF24">
         <v>4.219507705176107</v>
       </c>
-      <c r="AB24">
+      <c r="AG24">
         <v>4.30406509320417</v>
+      </c>
+      <c r="AH24">
+        <v>4.709530201312334</v>
       </c>
     </row>
     <row r="25">
@@ -2677,16 +3112,16 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T25">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U25">
         <v>0</v>
       </c>
       <c r="V25">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W25">
         <v>0.6931471805599453</v>
@@ -2695,16 +3130,34 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA25">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB25">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AC25">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AD25">
         <v>1.386294361119891</v>
       </c>
-      <c r="Z25">
+      <c r="AE25">
         <v>2.397895272798371</v>
       </c>
-      <c r="AA25">
+      <c r="AF25">
         <v>2.772588722239781</v>
       </c>
-      <c r="AB25">
+      <c r="AG25">
         <v>2.772588722239781</v>
+      </c>
+      <c r="AH25">
+        <v>4.248495242049359</v>
       </c>
     </row>
     <row r="26">
@@ -2769,34 +3222,52 @@
         <v>0</v>
       </c>
       <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="W26">
         <v>2.19722457733622</v>
       </c>
-      <c r="T26">
+      <c r="X26">
         <v>3.850147601710058</v>
       </c>
-      <c r="U26">
+      <c r="Y26">
         <v>4.499809670330265</v>
       </c>
-      <c r="V26">
+      <c r="Z26">
         <v>4.499809670330265</v>
       </c>
-      <c r="W26">
+      <c r="AA26">
         <v>4.605170185988092</v>
       </c>
-      <c r="X26">
+      <c r="AB26">
         <v>5.25227342804663</v>
       </c>
-      <c r="Y26">
+      <c r="AC26">
+        <v>5.805134968916488</v>
+      </c>
+      <c r="AD26">
         <v>5.961005339623274</v>
       </c>
-      <c r="Z26">
+      <c r="AE26">
         <v>6.142037405587356</v>
       </c>
-      <c r="AA26">
+      <c r="AF26">
         <v>6.54534966033442</v>
       </c>
-      <c r="AB26">
+      <c r="AG26">
         <v>6.612041034833092</v>
+      </c>
+      <c r="AH26">
+        <v>7.10085190894405</v>
       </c>
     </row>
     <row r="27">
@@ -2815,12 +3286,6 @@
           <t>Greenland</t>
         </is>
       </c>
-      <c r="D27">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
       <c r="F27">
         <v>0</v>
       </c>
@@ -2879,16 +3344,34 @@
         <v>0</v>
       </c>
       <c r="Y27">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AE27">
         <v>1.09861228866811</v>
       </c>
-      <c r="AA27">
+      <c r="AF27">
         <v>1.6094379124341</v>
       </c>
-      <c r="AB27">
+      <c r="AG27">
         <v>1.791759469228055</v>
+      </c>
+      <c r="AH27">
+        <v>2.397895272798371</v>
       </c>
     </row>
     <row r="28">
@@ -2953,34 +3436,52 @@
         <v>0</v>
       </c>
       <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+      <c r="U28">
+        <v>0</v>
+      </c>
+      <c r="V28">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="W28">
         <v>2.302585092994046</v>
       </c>
-      <c r="T28">
+      <c r="X28">
         <v>2.484906649788</v>
       </c>
-      <c r="U28">
+      <c r="Y28">
         <v>2.639057329615258</v>
       </c>
-      <c r="V28">
+      <c r="Z28">
         <v>2.833213344056216</v>
       </c>
-      <c r="W28">
+      <c r="AA28">
         <v>2.995732273553991</v>
       </c>
-      <c r="X28">
+      <c r="AB28">
         <v>3.49650756146648</v>
       </c>
-      <c r="Y28">
+      <c r="AC28">
+        <v>4.04305126783455</v>
+      </c>
+      <c r="AD28">
         <v>4.406719247264253</v>
       </c>
-      <c r="Z28">
+      <c r="AE28">
         <v>4.736198448394496</v>
       </c>
-      <c r="AA28">
+      <c r="AF28">
         <v>5.891644211825771</v>
       </c>
-      <c r="AB28">
+      <c r="AG28">
         <v>6.037870919922137</v>
+      </c>
+      <c r="AH28">
+        <v>6.766191714660351</v>
       </c>
     </row>
     <row r="29">
@@ -3048,31 +3549,49 @@
         <v>0</v>
       </c>
       <c r="T29">
+        <v>0</v>
+      </c>
+      <c r="U29">
+        <v>0</v>
+      </c>
+      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
+        <v>0</v>
+      </c>
+      <c r="X29">
         <v>1.6094379124341</v>
       </c>
-      <c r="U29">
+      <c r="Y29">
         <v>2.302585092994046</v>
       </c>
-      <c r="V29">
+      <c r="Z29">
         <v>2.564949357461537</v>
       </c>
-      <c r="W29">
+      <c r="AA29">
         <v>2.639057329615258</v>
       </c>
-      <c r="X29">
+      <c r="AB29">
         <v>2.995732273553991</v>
       </c>
-      <c r="Y29">
+      <c r="AC29">
+        <v>3.688879454113936</v>
+      </c>
+      <c r="AD29">
         <v>4.07753744390572</v>
       </c>
-      <c r="Z29">
+      <c r="AE29">
         <v>4.454347296253507</v>
       </c>
-      <c r="AA29">
+      <c r="AF29">
         <v>5.236441962829949</v>
       </c>
-      <c r="AB29">
+      <c r="AG29">
         <v>5.424950017481403</v>
+      </c>
+      <c r="AH29">
+        <v>6.20050917404269</v>
       </c>
     </row>
     <row r="30">
@@ -3137,34 +3656,52 @@
         <v>0</v>
       </c>
       <c r="S30">
+        <v>0</v>
+      </c>
+      <c r="T30">
+        <v>0</v>
+      </c>
+      <c r="U30">
+        <v>0</v>
+      </c>
+      <c r="V30">
+        <v>0</v>
+      </c>
+      <c r="W30">
         <v>1.09861228866811</v>
       </c>
-      <c r="T30">
+      <c r="X30">
         <v>2.94443897916644</v>
       </c>
-      <c r="U30">
+      <c r="Y30">
         <v>3.218875824868201</v>
       </c>
-      <c r="V30">
+      <c r="Z30">
         <v>3.555348061489414</v>
       </c>
-      <c r="W30">
+      <c r="AA30">
         <v>3.784189633918261</v>
       </c>
-      <c r="X30">
+      <c r="AB30">
         <v>4.51085950651685</v>
       </c>
-      <c r="Y30">
+      <c r="AC30">
+        <v>5.14166355650266</v>
+      </c>
+      <c r="AD30">
         <v>5.680172609017068</v>
       </c>
-      <c r="Z30">
+      <c r="AE30">
         <v>6.324358962381311</v>
       </c>
-      <c r="AA30">
+      <c r="AF30">
         <v>7.026426808699636</v>
       </c>
-      <c r="AB30">
+      <c r="AG30">
         <v>7.1929342212158</v>
+      </c>
+      <c r="AH30">
+        <v>7.976251943745623</v>
       </c>
     </row>
     <row r="31">
@@ -3229,34 +3766,52 @@
         <v>0</v>
       </c>
       <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
+      <c r="U31">
+        <v>0</v>
+      </c>
+      <c r="V31">
+        <v>0</v>
+      </c>
+      <c r="W31">
         <v>2.833213344056216</v>
       </c>
-      <c r="T31">
+      <c r="X31">
         <v>3.828641396489095</v>
       </c>
-      <c r="U31">
+      <c r="Y31">
         <v>4.189654742026425</v>
       </c>
-      <c r="V31">
+      <c r="Z31">
         <v>4.406719247264253</v>
       </c>
-      <c r="W31">
+      <c r="AA31">
         <v>4.454347296253507</v>
       </c>
-      <c r="X31">
+      <c r="AB31">
         <v>4.90527477843843</v>
       </c>
-      <c r="Y31">
+      <c r="AC31">
+        <v>5.198497031265826</v>
+      </c>
+      <c r="AD31">
         <v>5.525452939131783</v>
       </c>
-      <c r="Z31">
+      <c r="AE31">
         <v>5.802118375377063</v>
       </c>
-      <c r="AA31">
+      <c r="AF31">
         <v>6.378426183651587</v>
       </c>
-      <c r="AB31">
+      <c r="AG31">
         <v>6.47543271670409</v>
+      </c>
+      <c r="AH31">
+        <v>6.99117688712121</v>
       </c>
     </row>
     <row r="32">
@@ -3321,34 +3876,52 @@
         <v>0</v>
       </c>
       <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="U32">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="V32">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="W32">
         <v>2.772588722239781</v>
       </c>
-      <c r="T32">
+      <c r="X32">
         <v>3.091042453358316</v>
       </c>
-      <c r="U32">
+      <c r="Y32">
         <v>3.931825632724326</v>
       </c>
-      <c r="V32">
+      <c r="Z32">
         <v>4.343805421853684</v>
       </c>
-      <c r="W32">
+      <c r="AA32">
         <v>4.61512051684126</v>
       </c>
-      <c r="X32">
+      <c r="AB32">
         <v>4.969813299576001</v>
       </c>
-      <c r="Y32">
+      <c r="AC32">
+        <v>5.525452939131783</v>
+      </c>
+      <c r="AD32">
         <v>5.958424693029782</v>
       </c>
-      <c r="Z32">
+      <c r="AE32">
         <v>6.519147287940395</v>
       </c>
-      <c r="AA32">
+      <c r="AF32">
         <v>7.375882148215013</v>
       </c>
-      <c r="AB32">
+      <c r="AG32">
         <v>7.653969180478774</v>
+      </c>
+      <c r="AH32">
+        <v>8.458504195067558</v>
       </c>
     </row>
     <row r="33">
@@ -3413,34 +3986,52 @@
         <v>1.386294361119891</v>
       </c>
       <c r="S33">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="T33">
+        <v>4.382026634673881</v>
+      </c>
+      <c r="U33">
+        <v>5.393627546352362</v>
+      </c>
+      <c r="V33">
+        <v>6.270988431858299</v>
+      </c>
+      <c r="W33">
         <v>7.825245291431774</v>
       </c>
-      <c r="T33">
+      <c r="X33">
         <v>8.441822884391462</v>
       </c>
-      <c r="U33">
+      <c r="Y33">
         <v>9.129238770539141</v>
       </c>
-      <c r="V33">
+      <c r="Z33">
         <v>9.225228984469933</v>
       </c>
-      <c r="W33">
+      <c r="AA33">
         <v>9.430519533826377</v>
       </c>
-      <c r="X33">
+      <c r="AB33">
         <v>9.779114097696372</v>
       </c>
-      <c r="Y33">
+      <c r="AC33">
+        <v>10.11649995665088</v>
+      </c>
+      <c r="AD33">
         <v>10.35796502234825</v>
       </c>
-      <c r="Z33">
+      <c r="AE33">
         <v>10.6222050092076</v>
       </c>
-      <c r="AA33">
+      <c r="AF33">
         <v>11.0655127290543</v>
       </c>
-      <c r="AB33">
+      <c r="AG33">
         <v>11.14442371641643</v>
+      </c>
+      <c r="AH33">
+        <v>11.53017581837676</v>
       </c>
     </row>
     <row r="34">
@@ -3505,34 +4096,52 @@
         <v>0</v>
       </c>
       <c r="S34">
+        <v>0</v>
+      </c>
+      <c r="T34">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="U34">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="V34">
+        <v>1.386294361119891</v>
+      </c>
+      <c r="W34">
         <v>2.639057329615258</v>
       </c>
-      <c r="T34">
+      <c r="X34">
         <v>3.13549421592915</v>
       </c>
-      <c r="U34">
+      <c r="Y34">
         <v>3.737669618283368</v>
       </c>
-      <c r="V34">
+      <c r="Z34">
         <v>4.127134385045092</v>
       </c>
-      <c r="W34">
+      <c r="AA34">
         <v>4.127134385045092</v>
       </c>
-      <c r="X34">
+      <c r="AB34">
         <v>4.356708826689592</v>
       </c>
-      <c r="Y34">
+      <c r="AC34">
+        <v>4.605170185988092</v>
+      </c>
+      <c r="AD34">
         <v>4.897839799950911</v>
       </c>
-      <c r="Z34">
+      <c r="AE34">
         <v>5.068904202220232</v>
       </c>
-      <c r="AA34">
+      <c r="AF34">
         <v>5.720311776607412</v>
       </c>
-      <c r="AB34">
+      <c r="AG34">
         <v>5.811140992976701</v>
+      </c>
+      <c r="AH34">
+        <v>6.139884552226255</v>
       </c>
     </row>
     <row r="35">
@@ -3551,12 +4160,6 @@
           <t>Libya</t>
         </is>
       </c>
-      <c r="D35">
-        <v>0</v>
-      </c>
-      <c r="E35">
-        <v>0</v>
-      </c>
       <c r="F35">
         <v>0</v>
       </c>
@@ -3624,7 +4227,25 @@
         <v>0</v>
       </c>
       <c r="AB35">
-        <v>0.6931471805599453</v>
+        <v>0</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
+      <c r="AF35">
+        <v>0</v>
+      </c>
+      <c r="AG35">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AH35">
+        <v>2.19722457733622</v>
       </c>
     </row>
     <row r="36">
@@ -3643,12 +4264,6 @@
           <t>Liechtenstein</t>
         </is>
       </c>
-      <c r="D36">
-        <v>0</v>
-      </c>
-      <c r="E36">
-        <v>0</v>
-      </c>
       <c r="F36">
         <v>0</v>
       </c>
@@ -3689,16 +4304,16 @@
         <v>0</v>
       </c>
       <c r="S36">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T36">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U36">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V36">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W36">
         <v>0.6931471805599453</v>
@@ -3707,16 +4322,34 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="Y36">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z36">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA36">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB36">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AC36">
+        <v>2.079441541679836</v>
+      </c>
+      <c r="AD36">
         <v>3.931825632724326</v>
       </c>
-      <c r="Z36">
+      <c r="AE36">
         <v>3.367295829986474</v>
       </c>
-      <c r="AA36">
+      <c r="AF36">
         <v>3.951243718581428</v>
       </c>
-      <c r="AB36">
+      <c r="AG36">
         <v>3.951243718581428</v>
+      </c>
+      <c r="AH36">
+        <v>4.174387269895637</v>
       </c>
     </row>
     <row r="37">
@@ -3781,34 +4414,52 @@
         <v>0</v>
       </c>
       <c r="S37">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T37">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U37">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V37">
+        <v>0</v>
+      </c>
+      <c r="W37">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X37">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y37">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z37">
         <v>1.386294361119891</v>
       </c>
-      <c r="W37">
+      <c r="AA37">
         <v>1.386294361119891</v>
       </c>
-      <c r="X37">
+      <c r="AB37">
         <v>1.945910149055313</v>
       </c>
-      <c r="Y37">
+      <c r="AC37">
+        <v>2.70805020110221</v>
+      </c>
+      <c r="AD37">
         <v>3.332204510175204</v>
       </c>
-      <c r="Z37">
+      <c r="AE37">
         <v>3.891820298110626</v>
       </c>
-      <c r="AA37">
+      <c r="AF37">
         <v>5.236441962829949</v>
       </c>
-      <c r="AB37">
+      <c r="AG37">
         <v>5.545177444479562</v>
+      </c>
+      <c r="AH37">
+        <v>6.280395838960195</v>
       </c>
     </row>
     <row r="38">
@@ -3873,34 +4524,52 @@
         <v>0</v>
       </c>
       <c r="S38">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T38">
+        <v>0</v>
+      </c>
+      <c r="U38">
+        <v>0</v>
+      </c>
+      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X38">
         <v>1.09861228866811</v>
       </c>
-      <c r="U38">
+      <c r="Y38">
         <v>1.791759469228055</v>
       </c>
-      <c r="V38">
+      <c r="Z38">
         <v>2.079441541679836</v>
       </c>
-      <c r="W38">
+      <c r="AA38">
         <v>2.995732273553991</v>
       </c>
-      <c r="X38">
+      <c r="AB38">
         <v>3.555348061489414</v>
       </c>
-      <c r="Y38">
+      <c r="AC38">
+        <v>4.356708826689592</v>
+      </c>
+      <c r="AD38">
         <v>5.318119993844216</v>
       </c>
-      <c r="Z38">
+      <c r="AE38">
         <v>6.184148890937483</v>
       </c>
-      <c r="AA38">
+      <c r="AF38">
         <v>6.775366090936392</v>
       </c>
-      <c r="AB38">
+      <c r="AG38">
         <v>7.003065458786462</v>
+      </c>
+      <c r="AH38">
+        <v>7.595387278853972</v>
       </c>
     </row>
     <row r="39">
@@ -3965,34 +4634,52 @@
         <v>0</v>
       </c>
       <c r="S39">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T39">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U39">
+        <v>0</v>
+      </c>
+      <c r="V39">
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X39">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y39">
         <v>1.945910149055313</v>
       </c>
-      <c r="V39">
+      <c r="Z39">
         <v>2.19722457733622</v>
       </c>
-      <c r="W39">
+      <c r="AA39">
         <v>2.397895272798371</v>
       </c>
-      <c r="X39">
+      <c r="AB39">
         <v>2.94443897916644</v>
       </c>
-      <c r="Y39">
+      <c r="AC39">
+        <v>3.555348061489414</v>
+      </c>
+      <c r="AD39">
         <v>4.276666119016055</v>
       </c>
-      <c r="Z39">
+      <c r="AE39">
         <v>4.718498871295094</v>
       </c>
-      <c r="AA39">
+      <c r="AF39">
         <v>5.288267030694535</v>
       </c>
-      <c r="AB39">
+      <c r="AG39">
         <v>5.402677381872279</v>
+      </c>
+      <c r="AH39">
+        <v>5.988961416889864</v>
       </c>
     </row>
     <row r="40">
@@ -4057,34 +4744,52 @@
         <v>0</v>
       </c>
       <c r="S40">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T40">
+        <v>0</v>
+      </c>
+      <c r="U40">
+        <v>0</v>
+      </c>
+      <c r="V40">
+        <v>0</v>
+      </c>
+      <c r="W40">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X40">
         <v>1.09861228866811</v>
       </c>
-      <c r="U40">
+      <c r="Y40">
         <v>1.09861228866811</v>
       </c>
-      <c r="V40">
+      <c r="Z40">
         <v>1.791759469228055</v>
       </c>
-      <c r="W40">
+      <c r="AA40">
         <v>1.945910149055313</v>
       </c>
-      <c r="X40">
+      <c r="AB40">
         <v>2.079441541679836</v>
       </c>
-      <c r="Y40">
+      <c r="AC40">
+        <v>3.401197381662155</v>
+      </c>
+      <c r="AD40">
         <v>3.912023005428146</v>
       </c>
-      <c r="Z40">
+      <c r="AE40">
         <v>4.204692619390966</v>
       </c>
-      <c r="AA40">
+      <c r="AF40">
         <v>4.969813299576001</v>
       </c>
-      <c r="AB40">
+      <c r="AG40">
         <v>5.14166355650266</v>
+      </c>
+      <c r="AH40">
+        <v>6.354370040797351</v>
       </c>
     </row>
     <row r="41">
@@ -4103,12 +4808,6 @@
           <t>Monaco</t>
         </is>
       </c>
-      <c r="D41">
-        <v>0</v>
-      </c>
-      <c r="E41">
-        <v>0</v>
-      </c>
       <c r="F41">
         <v>0</v>
       </c>
@@ -4149,34 +4848,52 @@
         <v>0</v>
       </c>
       <c r="S41">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T41">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U41">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V41">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W41">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X41">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y41">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z41">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA41">
         <v>1.09861228866811</v>
       </c>
-      <c r="X41">
+      <c r="AB41">
         <v>1.09861228866811</v>
       </c>
-      <c r="Y41">
+      <c r="AC41">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="AD41">
         <v>2.079441541679836</v>
       </c>
-      <c r="Z41">
+      <c r="AE41">
         <v>2.484906649788</v>
       </c>
-      <c r="AA41">
+      <c r="AF41">
         <v>3.178053830347946</v>
       </c>
-      <c r="AB41">
+      <c r="AG41">
         <v>3.178053830347946</v>
+      </c>
+      <c r="AH41">
+        <v>3.912023005428146</v>
       </c>
     </row>
     <row r="42">
@@ -4247,28 +4964,46 @@
         <v>0</v>
       </c>
       <c r="U42">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V42">
+        <v>0</v>
+      </c>
+      <c r="W42">
+        <v>0</v>
+      </c>
+      <c r="X42">
+        <v>0</v>
+      </c>
+      <c r="Y42">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z42">
         <v>1.386294361119891</v>
       </c>
-      <c r="W42">
+      <c r="AA42">
         <v>1.386294361119891</v>
       </c>
-      <c r="X42">
+      <c r="AB42">
         <v>2.19722457733622</v>
       </c>
-      <c r="Y42">
+      <c r="AC42">
+        <v>3.178053830347946</v>
+      </c>
+      <c r="AD42">
         <v>3.433987204485146</v>
       </c>
-      <c r="Z42">
+      <c r="AE42">
         <v>3.912023005428146</v>
       </c>
-      <c r="AA42">
+      <c r="AF42">
         <v>4.700480365792417</v>
       </c>
-      <c r="AB42">
+      <c r="AG42">
         <v>4.836281906951478</v>
+      </c>
+      <c r="AH42">
+        <v>5.700443573390687</v>
       </c>
     </row>
     <row r="43">
@@ -4333,34 +5068,52 @@
         <v>0</v>
       </c>
       <c r="S43">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T43">
+        <v>0</v>
+      </c>
+      <c r="U43">
+        <v>0</v>
+      </c>
+      <c r="V43">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W43">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X43">
         <v>1.386294361119891</v>
       </c>
-      <c r="U43">
+      <c r="Y43">
         <v>1.6094379124341</v>
       </c>
-      <c r="V43">
+      <c r="Z43">
         <v>2.079441541679836</v>
       </c>
-      <c r="W43">
+      <c r="AA43">
         <v>2.079441541679836</v>
       </c>
-      <c r="X43">
+      <c r="AB43">
         <v>2.70805020110221</v>
       </c>
-      <c r="Y43">
+      <c r="AC43">
+        <v>2.995732273553991</v>
+      </c>
+      <c r="AD43">
         <v>3.58351893845611</v>
       </c>
-      <c r="Z43">
+      <c r="AE43">
         <v>3.931825632724326</v>
       </c>
-      <c r="AA43">
+      <c r="AF43">
         <v>5.003946305945459</v>
       </c>
-      <c r="AB43">
+      <c r="AG43">
         <v>5.181783550292085</v>
+      </c>
+      <c r="AH43">
+        <v>5.799092654460526</v>
       </c>
     </row>
     <row r="44">
@@ -4428,31 +5181,49 @@
         <v>0</v>
       </c>
       <c r="T44">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U44">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0</v>
+      </c>
+      <c r="X44">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y44">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z44">
         <v>1.945910149055313</v>
       </c>
-      <c r="W44">
+      <c r="AA44">
         <v>1.945910149055313</v>
       </c>
-      <c r="X44">
+      <c r="AB44">
         <v>2.564949357461537</v>
       </c>
-      <c r="Y44">
+      <c r="AC44">
+        <v>3.091042453358316</v>
+      </c>
+      <c r="AD44">
         <v>3.663561646129646</v>
       </c>
-      <c r="Z44">
+      <c r="AE44">
         <v>3.988984046564275</v>
       </c>
-      <c r="AA44">
+      <c r="AF44">
         <v>4.709530201312334</v>
       </c>
-      <c r="AB44">
+      <c r="AG44">
         <v>4.867534450455582</v>
+      </c>
+      <c r="AH44">
+        <v>5.135798437050262</v>
       </c>
     </row>
     <row r="45">
@@ -4535,16 +5306,34 @@
         <v>0</v>
       </c>
       <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0</v>
+      </c>
+      <c r="AB45">
+        <v>0</v>
+      </c>
+      <c r="AC45">
+        <v>0</v>
+      </c>
+      <c r="AD45">
         <v>1.09861228866811</v>
       </c>
-      <c r="Z45">
+      <c r="AE45">
         <v>2.639057329615258</v>
       </c>
-      <c r="AA45">
+      <c r="AF45">
         <v>3.401197381662155</v>
       </c>
-      <c r="AB45">
+      <c r="AG45">
         <v>3.970291913552122</v>
+      </c>
+      <c r="AH45">
+        <v>4.663439094112067</v>
       </c>
     </row>
     <row r="46">
@@ -4609,34 +5398,52 @@
         <v>0</v>
       </c>
       <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
         <v>3.663561646129646</v>
       </c>
-      <c r="T46">
+      <c r="X46">
         <v>4.859812404361672</v>
       </c>
-      <c r="U46">
+      <c r="Y46">
         <v>5.774551545544409</v>
       </c>
-      <c r="V46">
+      <c r="Z46">
         <v>5.948034989180646</v>
       </c>
-      <c r="W46">
+      <c r="AA46">
         <v>6.222576268071369</v>
       </c>
-      <c r="X46">
+      <c r="AB46">
         <v>6.690842277418564</v>
       </c>
-      <c r="Y46">
+      <c r="AC46">
+        <v>7.036148493750536</v>
+      </c>
+      <c r="AD46">
         <v>7.629003889652958</v>
       </c>
-      <c r="Z46">
+      <c r="AE46">
         <v>7.808323050391055</v>
       </c>
-      <c r="AA46">
+      <c r="AF46">
         <v>8.469682208745185</v>
       </c>
-      <c r="AB46">
+      <c r="AG46">
         <v>8.623533227187563</v>
+      </c>
+      <c r="AH46">
+        <v>9.441293350181875</v>
       </c>
     </row>
     <row r="47">
@@ -4701,34 +5508,52 @@
         <v>0</v>
       </c>
       <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W47">
         <v>3.49650756146648</v>
       </c>
-      <c r="T47">
+      <c r="X47">
         <v>4.736198448394496</v>
       </c>
-      <c r="U47">
+      <c r="Y47">
         <v>5.429345628954441</v>
       </c>
-      <c r="V47">
+      <c r="Z47">
         <v>6.063785208687608</v>
       </c>
-      <c r="W47">
+      <c r="AA47">
         <v>6.555356891810665</v>
       </c>
-      <c r="X47">
+      <c r="AB47">
         <v>6.904750769961838</v>
       </c>
-      <c r="Y47">
+      <c r="AC47">
+        <v>7.136483208590247</v>
+      </c>
+      <c r="AD47">
         <v>7.331714969726466</v>
       </c>
-      <c r="Z47">
+      <c r="AE47">
         <v>7.491087593534876</v>
       </c>
-      <c r="AA47">
+      <c r="AF47">
         <v>7.906915488678587</v>
       </c>
-      <c r="AB47">
+      <c r="AG47">
         <v>7.97349996402463</v>
+      </c>
+      <c r="AH47">
+        <v>8.432288684325794</v>
       </c>
     </row>
     <row r="48">
@@ -4793,34 +5618,52 @@
         <v>0</v>
       </c>
       <c r="S48">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T48">
+        <v>0</v>
+      </c>
+      <c r="U48">
+        <v>0</v>
+      </c>
+      <c r="V48">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W48">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X48">
         <v>1.791759469228055</v>
       </c>
-      <c r="U48">
+      <c r="Y48">
         <v>2.890371757896165</v>
       </c>
-      <c r="V48">
+      <c r="Z48">
         <v>3.258096538021482</v>
       </c>
-      <c r="W48">
+      <c r="AA48">
         <v>3.912023005428146</v>
       </c>
-      <c r="X48">
+      <c r="AB48">
         <v>4.23410650459726</v>
       </c>
-      <c r="Y48">
+      <c r="AC48">
+        <v>5.017279836814924</v>
+      </c>
+      <c r="AD48">
         <v>5.529429087511423</v>
       </c>
-      <c r="Z48">
+      <c r="AE48">
         <v>5.908082938168931</v>
       </c>
-      <c r="AA48">
+      <c r="AF48">
         <v>6.652863029353347</v>
       </c>
-      <c r="AB48">
+      <c r="AG48">
         <v>6.86484777797086</v>
+      </c>
+      <c r="AH48">
+        <v>7.703459047867175</v>
       </c>
     </row>
     <row r="49">
@@ -4885,34 +5728,52 @@
         <v>0</v>
       </c>
       <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
         <v>1.791759469228055</v>
       </c>
-      <c r="T49">
+      <c r="X49">
         <v>2.639057329615258</v>
       </c>
-      <c r="U49">
+      <c r="Y49">
         <v>3.433987204485146</v>
       </c>
-      <c r="V49">
+      <c r="Z49">
         <v>3.737669618283368</v>
       </c>
-      <c r="W49">
+      <c r="AA49">
         <v>4.0943445622221</v>
       </c>
-      <c r="X49">
+      <c r="AB49">
         <v>4.727387818712341</v>
       </c>
-      <c r="Y49">
+      <c r="AC49">
+        <v>5.505331535932362</v>
+      </c>
+      <c r="AD49">
         <v>6.107022887742255</v>
       </c>
-      <c r="Z49">
+      <c r="AE49">
         <v>6.668228248417403</v>
       </c>
-      <c r="AA49">
+      <c r="AF49">
         <v>7.630946580890459</v>
       </c>
-      <c r="AB49">
+      <c r="AG49">
         <v>8.005033344637111</v>
+      </c>
+      <c r="AH49">
+        <v>8.915163617762142</v>
       </c>
     </row>
     <row r="50">
@@ -4931,12 +5792,6 @@
           <t>Palestine</t>
         </is>
       </c>
-      <c r="D50">
-        <v>0</v>
-      </c>
-      <c r="E50">
-        <v>0</v>
-      </c>
       <c r="F50">
         <v>0</v>
       </c>
@@ -4980,31 +5835,49 @@
         <v>0</v>
       </c>
       <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50">
         <v>3.13549421592915</v>
       </c>
-      <c r="U50">
+      <c r="Y50">
         <v>3.258096538021482</v>
       </c>
-      <c r="V50">
+      <c r="Z50">
         <v>3.433987204485146</v>
       </c>
-      <c r="W50">
+      <c r="AA50">
         <v>3.433987204485146</v>
       </c>
-      <c r="X50">
+      <c r="AB50">
         <v>3.58351893845611</v>
       </c>
-      <c r="Y50">
+      <c r="AC50">
+        <v>3.663561646129646</v>
+      </c>
+      <c r="AD50">
         <v>3.737669618283368</v>
       </c>
-      <c r="Z50">
+      <c r="AE50">
         <v>3.871201010907891</v>
       </c>
-      <c r="AA50">
+      <c r="AF50">
         <v>4.110873864173311</v>
       </c>
-      <c r="AB50">
+      <c r="AG50">
         <v>4.143134726391533</v>
+      </c>
+      <c r="AH50">
+        <v>4.770684624465665</v>
       </c>
     </row>
     <row r="51">
@@ -5069,34 +5942,52 @@
         <v>0</v>
       </c>
       <c r="S51">
+        <v>0</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="W51">
         <v>1.6094379124341</v>
       </c>
-      <c r="T51">
+      <c r="X51">
         <v>2.302585092994046</v>
       </c>
-      <c r="U51">
+      <c r="Y51">
         <v>2.890371757896165</v>
       </c>
-      <c r="V51">
+      <c r="Z51">
         <v>3.465735902799727</v>
       </c>
-      <c r="W51">
+      <c r="AA51">
         <v>3.912023005428146</v>
       </c>
-      <c r="X51">
+      <c r="AB51">
         <v>4.499809670330265</v>
       </c>
-      <c r="Y51">
+      <c r="AC51">
+        <v>5.068904202220232</v>
+      </c>
+      <c r="AD51">
         <v>5.509388336627977</v>
       </c>
-      <c r="Z51">
+      <c r="AE51">
         <v>5.627621113690637</v>
       </c>
-      <c r="AA51">
+      <c r="AF51">
         <v>6.637258031284457</v>
       </c>
-      <c r="AB51">
+      <c r="AG51">
         <v>6.810142450115136</v>
+      </c>
+      <c r="AH51">
+        <v>7.716906135298388</v>
       </c>
     </row>
     <row r="52">
@@ -5161,34 +6052,52 @@
         <v>1.09861228866811</v>
       </c>
       <c r="S52">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="T52">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="U52">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="V52">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="W52">
         <v>1.945910149055313</v>
       </c>
-      <c r="T52">
+      <c r="X52">
         <v>2.639057329615258</v>
       </c>
-      <c r="U52">
+      <c r="Y52">
         <v>3.044522437723423</v>
       </c>
-      <c r="V52">
+      <c r="Z52">
         <v>3.044522437723423</v>
       </c>
-      <c r="W52">
+      <c r="AA52">
         <v>3.367295829986474</v>
       </c>
-      <c r="X52">
+      <c r="AB52">
         <v>3.871201010907891</v>
       </c>
-      <c r="Y52">
+      <c r="AC52">
+        <v>4.158883083359671</v>
+      </c>
+      <c r="AD52">
         <v>4.997212273764115</v>
       </c>
-      <c r="Z52">
+      <c r="AE52">
         <v>5.298317366548036</v>
       </c>
-      <c r="AA52">
+      <c r="AF52">
         <v>6.206575926724928</v>
       </c>
-      <c r="AB52">
+      <c r="AG52">
         <v>6.490723534502507</v>
+      </c>
+      <c r="AH52">
+        <v>7.757051142032013</v>
       </c>
     </row>
     <row r="53">
@@ -5207,12 +6116,6 @@
           <t>San Marino</t>
         </is>
       </c>
-      <c r="D53">
-        <v>0</v>
-      </c>
-      <c r="E53">
-        <v>0</v>
-      </c>
       <c r="F53">
         <v>0</v>
       </c>
@@ -5253,34 +6156,52 @@
         <v>0</v>
       </c>
       <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>0</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
         <v>2.772588722239781</v>
       </c>
-      <c r="T53">
+      <c r="X53">
         <v>3.178053830347946</v>
       </c>
-      <c r="U53">
+      <c r="Y53">
         <v>3.951243718581428</v>
       </c>
-      <c r="V53">
+      <c r="Z53">
         <v>4.110873864173311</v>
       </c>
-      <c r="W53">
+      <c r="AA53">
         <v>4.248495242049359</v>
       </c>
-      <c r="X53">
+      <c r="AB53">
         <v>4.394449154672439</v>
       </c>
-      <c r="Y53">
+      <c r="AC53">
+        <v>4.700480365792417</v>
+      </c>
+      <c r="AD53">
         <v>4.787491742782046</v>
       </c>
-      <c r="Z53">
+      <c r="AE53">
         <v>4.976733742420574</v>
       </c>
-      <c r="AA53">
+      <c r="AF53">
         <v>5.236441962829949</v>
       </c>
-      <c r="AB53">
+      <c r="AG53">
         <v>5.236441962829949</v>
+      </c>
+      <c r="AH53">
+        <v>5.442417710521793</v>
       </c>
     </row>
     <row r="54">
@@ -5348,31 +6269,49 @@
         <v>0</v>
       </c>
       <c r="T54">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y54">
         <v>1.6094379124341</v>
       </c>
-      <c r="V54">
+      <c r="Z54">
         <v>2.564949357461537</v>
       </c>
-      <c r="W54">
+      <c r="AA54">
         <v>2.995732273553991</v>
       </c>
-      <c r="X54">
+      <c r="AB54">
         <v>3.58351893845611</v>
       </c>
-      <c r="Y54">
+      <c r="AC54">
+        <v>4.02535169073515</v>
+      </c>
+      <c r="AD54">
         <v>4.430816798843313</v>
       </c>
-      <c r="Z54">
+      <c r="AE54">
         <v>4.77912349311153</v>
       </c>
-      <c r="AA54">
+      <c r="AF54">
         <v>5.521460917862246</v>
       </c>
-      <c r="AB54">
+      <c r="AG54">
         <v>5.953243334287785</v>
+      </c>
+      <c r="AH54">
+        <v>6.803505257608338</v>
       </c>
     </row>
     <row r="55">
@@ -5440,31 +6379,49 @@
         <v>0</v>
       </c>
       <c r="T55">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U55">
+        <v>0</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>0</v>
+      </c>
+      <c r="X55">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y55">
         <v>2.079441541679836</v>
       </c>
-      <c r="V55">
+      <c r="Z55">
         <v>2.397895272798371</v>
       </c>
-      <c r="W55">
+      <c r="AA55">
         <v>2.833213344056216</v>
       </c>
-      <c r="X55">
+      <c r="AB55">
         <v>3.49650756146648</v>
       </c>
-      <c r="Y55">
+      <c r="AC55">
+        <v>4.127134385045092</v>
+      </c>
+      <c r="AD55">
         <v>4.584967478670572</v>
       </c>
-      <c r="Z55">
+      <c r="AE55">
         <v>4.828313737302302</v>
       </c>
-      <c r="AA55">
+      <c r="AF55">
         <v>5.323009979138408</v>
       </c>
-      <c r="AB55">
+      <c r="AG55">
         <v>5.37989735354046</v>
+      </c>
+      <c r="AH55">
+        <v>5.897153867636741</v>
       </c>
     </row>
     <row r="56">
@@ -5532,31 +6489,49 @@
         <v>0</v>
       </c>
       <c r="T56">
+        <v>0</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>0</v>
+      </c>
+      <c r="X56">
         <v>2.079441541679836</v>
       </c>
-      <c r="U56">
+      <c r="Y56">
         <v>3.258096538021482</v>
       </c>
-      <c r="V56">
+      <c r="Z56">
         <v>3.555348061489414</v>
       </c>
-      <c r="W56">
+      <c r="AA56">
         <v>4.499809670330265</v>
       </c>
-      <c r="X56">
+      <c r="AB56">
         <v>4.955827057601261</v>
       </c>
-      <c r="Y56">
+      <c r="AC56">
+        <v>5.393627546352362</v>
+      </c>
+      <c r="AD56">
         <v>5.62040086571715</v>
       </c>
-      <c r="Z56">
+      <c r="AE56">
         <v>5.768320995793772</v>
       </c>
-      <c r="AA56">
+      <c r="AF56">
         <v>6.093569770045136</v>
       </c>
-      <c r="AB56">
+      <c r="AG56">
         <v>6.270988431858299</v>
+      </c>
+      <c r="AH56">
+        <v>6.688354713946762</v>
       </c>
     </row>
     <row r="57">
@@ -5621,34 +6596,52 @@
         <v>0.6931471805599453</v>
       </c>
       <c r="S57">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="T57">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="U57">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="V57">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="W57">
         <v>3.58351893845611</v>
       </c>
-      <c r="T57">
+      <c r="X57">
         <v>4.624972813284271</v>
       </c>
-      <c r="U57">
+      <c r="Y57">
         <v>5.568344503761097</v>
       </c>
-      <c r="V57">
+      <c r="Z57">
         <v>5.87493073085203</v>
       </c>
-      <c r="W57">
+      <c r="AA57">
         <v>6.216606101084865</v>
       </c>
-      <c r="X57">
+      <c r="AB57">
         <v>6.703188113240863</v>
       </c>
-      <c r="Y57">
+      <c r="AC57">
+        <v>6.947937068614969</v>
+      </c>
+      <c r="AD57">
         <v>7.10085190894405</v>
       </c>
-      <c r="Z57">
+      <c r="AE57">
         <v>7.277247726631484</v>
       </c>
-      <c r="AA57">
+      <c r="AF57">
         <v>7.630461261783627</v>
       </c>
-      <c r="AB57">
+      <c r="AG57">
         <v>7.76046702921342</v>
+      </c>
+      <c r="AH57">
+        <v>8.397508348470257</v>
       </c>
     </row>
     <row r="58">
@@ -5737,10 +6730,28 @@
         <v>0</v>
       </c>
       <c r="AA58">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="AB58">
-        <v>0.6931471805599453</v>
+        <v>0</v>
+      </c>
+      <c r="AC58">
+        <v>0</v>
+      </c>
+      <c r="AD58">
+        <v>0</v>
+      </c>
+      <c r="AE58">
+        <v>0</v>
+      </c>
+      <c r="AF58">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AG58">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AH58">
+        <v>2.397895272798371</v>
       </c>
     </row>
     <row r="59">
@@ -5805,34 +6816,52 @@
         <v>0</v>
       </c>
       <c r="S59">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T59">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U59">
+        <v>0</v>
+      </c>
+      <c r="V59">
+        <v>0</v>
+      </c>
+      <c r="W59">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="X59">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y59">
         <v>1.791759469228055</v>
       </c>
-      <c r="V59">
+      <c r="Z59">
         <v>1.945910149055313</v>
       </c>
-      <c r="W59">
+      <c r="AA59">
         <v>2.079441541679836</v>
       </c>
-      <c r="X59">
+      <c r="AB59">
         <v>2.833213344056216</v>
       </c>
-      <c r="Y59">
+      <c r="AC59">
+        <v>3.044522437723423</v>
+      </c>
+      <c r="AD59">
         <v>3.401197381662155</v>
       </c>
-      <c r="Z59">
+      <c r="AE59">
         <v>3.688879454113936</v>
       </c>
-      <c r="AA59">
+      <c r="AF59">
         <v>4.74493212836325</v>
       </c>
-      <c r="AB59">
+      <c r="AG59">
         <v>4.787491742782046</v>
+      </c>
+      <c r="AH59">
+        <v>5.89440283426485</v>
       </c>
     </row>
     <row r="60">
@@ -5906,25 +6935,43 @@
         <v>0</v>
       </c>
       <c r="V60">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W60">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="X60">
+        <v>0</v>
+      </c>
+      <c r="Y60">
+        <v>0</v>
+      </c>
+      <c r="Z60">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA60">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB60">
         <v>1.791759469228055</v>
       </c>
-      <c r="Y60">
+      <c r="AC60">
+        <v>2.94443897916644</v>
+      </c>
+      <c r="AD60">
         <v>4.59511985013459</v>
       </c>
-      <c r="Z60">
+      <c r="AE60">
         <v>5.886104031450156</v>
       </c>
-      <c r="AA60">
+      <c r="AF60">
         <v>7.333023014386481</v>
       </c>
-      <c r="AB60">
+      <c r="AG60">
         <v>7.535296702444088</v>
+      </c>
+      <c r="AH60">
+        <v>9.289890650734192</v>
       </c>
     </row>
     <row r="61">
@@ -5989,57 +7036,75 @@
         <v>0</v>
       </c>
       <c r="S61">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="T61">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U61">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V61">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W61">
         <v>0.6931471805599453</v>
       </c>
       <c r="X61">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Y61">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="Z61">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA61">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB61">
         <v>1.386294361119891</v>
       </c>
-      <c r="Y61">
+      <c r="AC61">
+        <v>1.791759469228055</v>
+      </c>
+      <c r="AD61">
         <v>2.70805020110221</v>
       </c>
-      <c r="Z61">
+      <c r="AE61">
         <v>3.295836866004329</v>
       </c>
-      <c r="AA61">
+      <c r="AF61">
         <v>4.584967478670572</v>
       </c>
-      <c r="AB61">
+      <c r="AG61">
         <v>4.736198448394496</v>
+      </c>
+      <c r="AH61">
+        <v>6.309918278226516</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>XKX</t>
+          <t>USA</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>科索沃</t>
+          <t>美國</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Kosovo</t>
+          <t>United States of America</t>
         </is>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>27659597.30520719</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>17.13548336150712</v>
       </c>
       <c r="F62">
         <v>0</v>
@@ -6051,80 +7116,98 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>0</v>
+        <v>1.09861228866811</v>
       </c>
       <c r="J62">
-        <v>0</v>
+        <v>1.09861228866811</v>
       </c>
       <c r="K62">
-        <v>0</v>
+        <v>2.19722457733622</v>
       </c>
       <c r="L62">
-        <v>0</v>
+        <v>2.484906649788</v>
       </c>
       <c r="M62">
-        <v>0</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="N62">
-        <v>0</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="O62">
-        <v>0</v>
+        <v>2.564949357461537</v>
       </c>
       <c r="P62">
-        <v>0</v>
+        <v>2.639057329615258</v>
       </c>
       <c r="Q62">
-        <v>0</v>
+        <v>2.772588722239781</v>
       </c>
       <c r="R62">
-        <v>0</v>
+        <v>2.772588722239781</v>
       </c>
       <c r="S62">
-        <v>0</v>
+        <v>2.772588722239781</v>
       </c>
       <c r="T62">
-        <v>0</v>
+        <v>3.58351893845611</v>
       </c>
       <c r="U62">
-        <v>0</v>
+        <v>3.58351893845611</v>
       </c>
       <c r="V62">
-        <v>0</v>
+        <v>4.110873864173311</v>
       </c>
       <c r="W62">
-        <v>0</v>
+        <v>4.859812404361672</v>
       </c>
       <c r="X62">
-        <v>1.09861228866811</v>
+        <v>5.837730447165939</v>
       </c>
       <c r="Y62">
-        <v>2.995732273553991</v>
+        <v>6.628041376179533</v>
       </c>
       <c r="Z62">
-        <v>3.091042453358316</v>
+        <v>6.946975992135418</v>
       </c>
       <c r="AA62">
-        <v>4.127134385045092</v>
+        <v>7.188412736496954</v>
       </c>
       <c r="AB62">
-        <v>4.158883083359671</v>
+        <v>7.684783943522785</v>
+      </c>
+      <c r="AC62">
+        <v>8.24354550792826</v>
+      </c>
+      <c r="AD62">
+        <v>8.779095810880531</v>
+      </c>
+      <c r="AE62">
+        <v>9.572689189010719</v>
+      </c>
+      <c r="AF62">
+        <v>10.7449900809517</v>
+      </c>
+      <c r="AG62">
+        <v>10.91761254875864</v>
+      </c>
+      <c r="AH62">
+        <v>12.00953451037694</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>VAT</t>
+          <t>XKX</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>梵蒂岡</t>
+          <t>科索沃</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Vatican</t>
+          <t>Kosovo</t>
         </is>
       </c>
       <c r="F63">
@@ -6170,47 +7253,65 @@
         <v>0</v>
       </c>
       <c r="T63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="U63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="V63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="X63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="Y63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="Z63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="AA63">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="AB63">
-        <v>1.6094379124341</v>
+        <v>1.09861228866811</v>
+      </c>
+      <c r="AC63">
+        <v>2.302585092994046</v>
+      </c>
+      <c r="AD63">
+        <v>2.995732273553991</v>
+      </c>
+      <c r="AE63">
+        <v>3.091042453358316</v>
+      </c>
+      <c r="AF63">
+        <v>4.127134385045092</v>
+      </c>
+      <c r="AG63">
+        <v>4.158883083359671</v>
+      </c>
+      <c r="AH63">
+        <v>4.672828834461906</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>JEY</t>
+          <t>VAT</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>澤西島</t>
+          <t>梵蒂岡</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Jersey</t>
+          <t>Vatican</t>
         </is>
       </c>
       <c r="F64">
@@ -6262,111 +7363,251 @@
         <v>0</v>
       </c>
       <c r="V64">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="W64">
-        <v>0.6931471805599453</v>
+        <v>0</v>
       </c>
       <c r="X64">
         <v>0.6931471805599453</v>
       </c>
       <c r="Y64">
-        <v>1.791759469228055</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="Z64">
-        <v>2.397895272798371</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AA64">
-        <v>2.833213344056216</v>
+        <v>0.6931471805599453</v>
       </c>
       <c r="AB64">
-        <v>2.833213344056216</v>
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AC64">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AD64">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AE64">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AF64">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AG64">
+        <v>1.6094379124341</v>
+      </c>
+      <c r="AH64">
+        <v>1.945910149055313</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
+          <t>JEY</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>澤西島</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>Jersey</t>
+        </is>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+      <c r="T65">
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <v>0</v>
+      </c>
+      <c r="V65">
+        <v>0</v>
+      </c>
+      <c r="W65">
+        <v>0</v>
+      </c>
+      <c r="X65">
+        <v>0</v>
+      </c>
+      <c r="Y65">
+        <v>0</v>
+      </c>
+      <c r="Z65">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA65">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB65">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AC65">
+        <v>1.09861228866811</v>
+      </c>
+      <c r="AD65">
+        <v>1.791759469228055</v>
+      </c>
+      <c r="AE65">
+        <v>2.397895272798371</v>
+      </c>
+      <c r="AF65">
+        <v>2.833213344056216</v>
+      </c>
+      <c r="AG65">
+        <v>2.833213344056216</v>
+      </c>
+      <c r="AH65">
+        <v>4.406719247264253</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
           <t>GGY</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
+      <c r="B66" t="inlineStr">
         <is>
           <t>根西島</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="C66" t="inlineStr">
         <is>
           <t>Guernsey</t>
         </is>
       </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-      <c r="I65">
-        <v>0</v>
-      </c>
-      <c r="J65">
-        <v>0</v>
-      </c>
-      <c r="K65">
-        <v>0</v>
-      </c>
-      <c r="L65">
-        <v>0</v>
-      </c>
-      <c r="M65">
-        <v>0</v>
-      </c>
-      <c r="N65">
-        <v>0</v>
-      </c>
-      <c r="O65">
-        <v>0</v>
-      </c>
-      <c r="P65">
-        <v>0</v>
-      </c>
-      <c r="Q65">
-        <v>0</v>
-      </c>
-      <c r="R65">
-        <v>0</v>
-      </c>
-      <c r="S65">
-        <v>0</v>
-      </c>
-      <c r="T65">
-        <v>0</v>
-      </c>
-      <c r="U65">
-        <v>0</v>
-      </c>
-      <c r="V65">
-        <v>0.6931471805599453</v>
-      </c>
-      <c r="W65">
-        <v>0.6931471805599453</v>
-      </c>
-      <c r="X65">
-        <v>0.6931471805599453</v>
-      </c>
-      <c r="Y65">
-        <v>0.6931471805599453</v>
-      </c>
-      <c r="Z65">
-        <v>0.6931471805599453</v>
-      </c>
-      <c r="AA65">
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <v>0</v>
+      </c>
+      <c r="J66">
+        <v>0</v>
+      </c>
+      <c r="K66">
+        <v>0</v>
+      </c>
+      <c r="L66">
+        <v>0</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+      <c r="N66">
+        <v>0</v>
+      </c>
+      <c r="O66">
+        <v>0</v>
+      </c>
+      <c r="P66">
+        <v>0</v>
+      </c>
+      <c r="Q66">
+        <v>0</v>
+      </c>
+      <c r="R66">
+        <v>0</v>
+      </c>
+      <c r="S66">
+        <v>0</v>
+      </c>
+      <c r="T66">
+        <v>0</v>
+      </c>
+      <c r="U66">
+        <v>0</v>
+      </c>
+      <c r="V66">
+        <v>0</v>
+      </c>
+      <c r="W66">
+        <v>0</v>
+      </c>
+      <c r="X66">
+        <v>0</v>
+      </c>
+      <c r="Y66">
+        <v>0</v>
+      </c>
+      <c r="Z66">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AA66">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AB66">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AC66">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AD66">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AE66">
+        <v>0.6931471805599453</v>
+      </c>
+      <c r="AF66">
         <v>3.044522437723423</v>
       </c>
-      <c r="AB65">
+      <c r="AG66">
         <v>3.178053830347946</v>
+      </c>
+      <c r="AH66">
+        <v>4.110873864173311</v>
       </c>
     </row>
   </sheetData>

</xml_diff>